<commit_message>
update report day 11/09/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,174 +27,198 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://www.facebook.com/tintuc247247/posts/pfbid0qXCpsK1wePx1kMpz172kpctboafHY2sb1nigNcUaGrHG5zHj5b3djWWH9546AkV2l</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/pfbid0t2fxmGKkEUjTkv9YLtiGC1wp9uC475pxoSCnFwRpXgVkN9qBZ58rRZXg4xxVoyg7l</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/pfbid0sUg2AeYgP3KyL9pPm9uo8AeNYdDuoZ1BRne1RxQpMTjoex3nfgUqzf94y7M2Hnojl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thienluong25/posts/pfbid0eL4RUesZR5ZoXfbBeSfm282jBxGG4W9cwKTQ2MPRTkrqnzUS2V7USYDPKuto7Vqdl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/pfbid0CqFCvL1LMv9zmN31jNyShspZ891RoTpXXrcRXLuDGfjfsuZd5aNLGRe3k1hzcDzMl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/pfbid023yC8b9a16TKKWBaswWwYCkqqzreDAsuyKTAAqdiUS6vMPgBzP4QwPQRy51Jc5Pv9l</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/pfbid02zf6EmS6GfDiRx69H1F9S15tFw441wpgCZHNntUmrSwB7y3MzC8oKHqosnxuxwVo8l</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/pfbid0LABVyg3Jox3fhHUhTWcxBPUv4U1cEveE8gAQp4ThcWjezec1u54kReZVKn5BvEXMl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/vtcnewsvn/posts/pfbid0315t5ECn1ZZZ3Ck6MPnoutZF3GVPM2ksGXiEpQax5nTm6RvBTi8haqQSEHQE2knGtl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/530451602869695?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/530426959538826?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/530395056208683?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/530061839575338?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529924432922412?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529795102935345?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529434092971446?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529401232974732?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529290529652469?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906862068134959?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906821031472396?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906795248141641?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906755858145580?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906713588149807?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906498454837987?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906464424841390?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906431548178011?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906362788184887?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906281758192990?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906190748202091?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/906053778215788?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905815538239612?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905810561573443?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905717448249421?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905627501591749?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905615171592982?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905550994932733?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905501938270972?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905455528275613?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905424668278699?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905414514946381?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905236694964163?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905156364972196?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905191301635369?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905125894975243?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/905067401647759?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904984588322707?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904848145003018?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904558588365307?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904469478374218?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904382265049606?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/chantroimoimedia/posts/904371345050698?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/viettan/posts/930176689152339?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/viettan/posts/930082639161744?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/viettan/posts/930046929165315?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/viettan/posts/929800342523307?ref=embed_post</t>
+    <t>https://www.facebook.com/tintuc247247/posts/551017464146442?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550348527546669?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550296610885194?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550273524220836?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550238730890982?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550196254228563?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550135510901304?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/550103910904464?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/549663904281798?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/549037224344466?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951323963704278?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951290430374298?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951277507042257?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951228030380538?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951189673717707?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951206137049394?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/viettan/posts/951097240393617?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/548997581015097?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/548384204409768?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/548162901098565?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/547607714487417?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/547534014494787?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/547492717832250?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/547435414504647?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/547008471214008?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/546720491242806?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/546241654624023?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/546667031248152?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/546015024646686?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/544363144811874?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/544208908160631?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/543981024850086?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/543632044884984?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/542884504959738?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/543345014913687?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/541787591736096?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/541077328473789?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/541050455143143?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/541016741813181?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540672368514285?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540592938522228?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540528238528698?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540484361866419?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540404175207771?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/540351851879670?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/539822461932609?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/538559818725540?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/538470915401097?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/537936418787880?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/537819172132938?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/537130798868442?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/536691072245748?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/534648769116645?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/533978645850324?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/927913389363160?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/927586832729149?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/927507442737088?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/927484586072707?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/927460866075079?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/926992656121900?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/926810119473487?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/926511922836640?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chantroimoimedia/posts/926423066178859?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -218,7 +242,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,7 +250,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -680,12 +704,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -810,8 +834,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1347,10 +1374,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A56"/>
+  <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1361,7 +1388,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1386,7 +1413,7 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1507,132 +1534,177 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data day 20/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="13545" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/964043959089937?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963780079116325?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963721785788821?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963387679155565?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963266382501028?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963193552508311?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963055725855427?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963038832523783?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/963026039191729?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/962881379206195?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988854093279371?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988882469943200?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/989049856593128?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/987988396699274?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988029190028528?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/987443800087067?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988867133278067?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988127853351995?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/988082110023236?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/986517283513052?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/986576653507115?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/986622820169165?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/986570580174389?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1251,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1195,6 +1264,121 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update data day 21/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>link</t>
   </si>
@@ -99,6 +99,297 @@
   </si>
   <si>
     <t>https://www.facebook.com/thongtinchinhphu/posts/986570580174389?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/986186283546152?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985610296937084?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985437616954352?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985133396984774?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985123206985793?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985004743664306?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/985110820320365?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/984913873673393?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/984827680348679?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/984231030408344?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/984220663742714?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/983512893813491?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/983100937188020?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/983244920506955?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/982341943930586?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/982678903896890?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981956287302485?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981804130651034?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981741710657276?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981790440652403?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981610670670380?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981385857359528?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981043764060404?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981046457393468?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981039514060829?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/980992030732244?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/981154850715962?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/881783077373891?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/881654814053384?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/881313624087503?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/881315360753996?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/881314527420746?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880753314143534?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880752837476915?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880636624155203?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880635234155342?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880634607488738?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880519440833588?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880251330860399?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880249834193882?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880249220860610?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880135807538618?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/880018180883714?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879993847552814?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879975050888027?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879828897569309?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879825997569599?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879826507569548?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879494384269427?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879491310936401?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879227444296121?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879226637629535?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879225547629644?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879224727629726?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879223810963151?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879102794308586?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879101247642074?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/879099590975573?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/878804271005105?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/878430701042462?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/878554227696776?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/878327984386067?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877943121091220?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877839401101592?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877837871101745?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877593647792834?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877592734459592?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877591714459694?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877590381126494?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/877588994459966?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876932711192261?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876934391192093?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876933934525472?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876933481192184?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876931847859014?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876842871201245?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876842197867979?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876413567910842?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876841547868044?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876236571261875?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876235047928694?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876234261262106?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876233224595543?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876024484616417?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/876022357949963?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/875568004662065?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/875568791328653?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/875359594682906?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/875360158016183?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/875359028016296?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874848064734059?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874847301400802?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874846491400883?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874593441426188?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874422351443297?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874421478110051?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thoisuvtv/posts/874420481443484?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -1251,10 +1542,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1379,6 +1670,491 @@
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update data day 22/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,369 +27,255 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://www.facebook.com/K14vn/posts/964043959089937?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963780079116325?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963721785788821?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963387679155565?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963266382501028?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963193552508311?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963055725855427?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963038832523783?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/963026039191729?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/962881379206195?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988854093279371?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988882469943200?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/989049856593128?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/987988396699274?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988029190028528?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/987443800087067?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988867133278067?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988127853351995?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/988082110023236?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/986517283513052?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/986576653507115?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/986622820169165?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/986570580174389?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/986186283546152?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985610296937084?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985437616954352?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985133396984774?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985123206985793?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985004743664306?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/985110820320365?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/984913873673393?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/984827680348679?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/984231030408344?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/984220663742714?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/983512893813491?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/983100937188020?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/983244920506955?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/982341943930586?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/982678903896890?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981956287302485?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981804130651034?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981741710657276?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981790440652403?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981610670670380?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981385857359528?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981043764060404?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981046457393468?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981039514060829?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/980992030732244?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/981154850715962?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/881783077373891?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/881654814053384?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/881313624087503?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/881315360753996?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/881314527420746?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880753314143534?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880752837476915?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880636624155203?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880635234155342?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880634607488738?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880519440833588?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880251330860399?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880249834193882?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880249220860610?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880135807538618?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/880018180883714?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879993847552814?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879975050888027?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879828897569309?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879825997569599?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879826507569548?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879494384269427?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879491310936401?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879227444296121?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879226637629535?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879225547629644?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879224727629726?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879223810963151?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879102794308586?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879101247642074?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/879099590975573?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/878804271005105?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/878430701042462?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/878554227696776?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/878327984386067?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877943121091220?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877839401101592?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877837871101745?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877593647792834?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877592734459592?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877591714459694?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877590381126494?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/877588994459966?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876932711192261?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876934391192093?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876933934525472?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876933481192184?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876931847859014?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876842871201245?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876842197867979?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876413567910842?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876841547868044?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876236571261875?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876235047928694?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876234261262106?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876233224595543?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876024484616417?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/876022357949963?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/875568004662065?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/875568791328653?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/875359594682906?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/875360158016183?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/875359028016296?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874848064734059?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874847301400802?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874846491400883?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874593441426188?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874422351443297?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874421478110051?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thoisuvtv/posts/874420481443484?ref=embed_post</t>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953965943432084?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953937886768223?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953892656772746?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953881060107239?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953823086779703?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953819660113379?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953813353447343?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/953804186781593?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/952364056925606?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/952328523595826?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/952283433600335?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/952012636960748?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951947586967253?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951497913678887?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951428257019186?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951319813696697?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951289523699726?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951239810371364?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951229007039111?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951224637039548?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/951208900374455?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950884390406906?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950857003742978?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950828540412491?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950761407085871?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950727830422562?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950655273763151?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950605607101451?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950542900441055?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950333430462002?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/950116753817003?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949900920505253?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949860963842582?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949824407179571?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949773443851334?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949726607189351?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949608467201165?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949548650540480?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949268080568537?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949216987240313?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/949152517246760?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948982143930464?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948946657267346?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948758417286170?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948486053980073?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948473257314686?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948422930653052?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948402717321740?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948366913991987?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948353727326639?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948159430679402?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/948340980661247?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/947570744071604?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/947540134074665?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/947515924077086?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/947474560747889?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/947111760784169?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946879040807441?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946715844157094?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946454654183213?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946433690851976?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946042294224449?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/946018254226853?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945969007565111?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945891494239529?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945795877582424?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945730104255668?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945661177595894?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945576374271041?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945526934275985?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945497520945593?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945483034280375?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945189117643100?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945220284306650?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/945088670986478?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944944611000884?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944915534337125?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944829941012351?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944811187680893?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944720404356638?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944714437690568?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/congdongvnexpress/posts/944607861034559?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +891,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1542,10 +1431,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A121"/>
+  <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1631,7 +1520,7 @@
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1897,262 +1786,77 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>120</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update report day 25/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,255 +27,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953965943432084?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953937886768223?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953892656772746?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953881060107239?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953823086779703?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953819660113379?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953813353447343?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/953804186781593?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/952364056925606?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/952328523595826?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/952283433600335?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/952012636960748?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951947586967253?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951497913678887?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951428257019186?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951319813696697?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951289523699726?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951239810371364?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951229007039111?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951224637039548?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/951208900374455?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950884390406906?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950857003742978?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950828540412491?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950761407085871?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950727830422562?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950655273763151?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950605607101451?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950542900441055?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950333430462002?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/950116753817003?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949900920505253?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949860963842582?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949824407179571?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949773443851334?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949726607189351?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949608467201165?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949548650540480?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949268080568537?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949216987240313?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/949152517246760?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948982143930464?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948946657267346?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948758417286170?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948486053980073?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948473257314686?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948422930653052?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948402717321740?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948366913991987?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948353727326639?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948159430679402?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/948340980661247?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/947570744071604?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/947540134074665?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/947515924077086?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/947474560747889?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/947111760784169?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946879040807441?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946715844157094?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946454654183213?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946433690851976?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946042294224449?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/946018254226853?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945969007565111?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945891494239529?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945795877582424?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945730104255668?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945661177595894?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945576374271041?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945526934275985?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945497520945593?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945483034280375?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945189117643100?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945220284306650?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/945088670986478?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944944611000884?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944915534337125?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944829941012351?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944811187680893?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944720404356638?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944714437690568?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/congdongvnexpress/posts/944607861034559?ref=embed_post</t>
+    <t>https://www.facebook.com/K14vn/posts/967228682104798?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967221998772133?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967207705440229?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967186722108994?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967169058777427?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967148892112777?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967114128782920?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967100842117582?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967043255456674?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967033045457695?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/967009495460050?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966942885466711?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966706425490357?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966653402162326?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966566715504328?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966521775508822?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966476808846652?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966388225522177?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966375708856762?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966335782194088?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966306918863641?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966263705534629?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/965422742285392?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966245622203104?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966243385536661?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966202212207445?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966189408875392?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966167398877593?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/966134648880868?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/965910925569907?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/965679468926386?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/965634952264171?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/965586232269043?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -891,11 +744,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1431,10 +1281,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A84"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1520,7 +1370,7 @@
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1607,256 +1457,6 @@
     <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update report day 30/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>link</t>
   </si>
@@ -129,6 +129,117 @@
   </si>
   <si>
     <t>https://www.facebook.com/K14vn/posts/965586232269043?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969491778545155?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969471348547198?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969461055214894?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969456385215361?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969449648549368?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969421088552224?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969417051885961?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969402445220755?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969392405221759?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969383878555945?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969158118578521?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/969022685258731?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/968831421944524?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/968728055288194?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/968366765324323?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993967199434727?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993892006108913?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993843276113786?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993793022785478?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993316289499818?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993150319516415?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993217509509696?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/992697889561658?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/992705136227600?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/993099756188138?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/992340396264074?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/992190762945704?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991932829638164?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/992455706252543?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991791036319010?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991721729659274?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991608156337298?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991108859720561?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/991096326388481?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/990926029738844?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/990618286436285?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/thongtinchinhphu/posts/990373226460791?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -141,12 +252,24 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -614,138 +737,144 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1281,10 +1410,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1454,12 +1583,200 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="34" s="1" customFormat="1" spans="1:1">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A34" r:id="rId1" display="https://www.facebook.com/K14vn/posts/965586232269043?ref=embed_post"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
update report TIIS day 8/11/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/url_fake.xlsx
+++ b/Data/Draft/url_fake.xlsx
@@ -27,219 +27,225 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://www.facebook.com/K14vn/posts/967228682104798?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967221998772133?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967207705440229?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967186722108994?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967169058777427?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967148892112777?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967114128782920?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967100842117582?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967043255456674?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967033045457695?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/967009495460050?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966942885466711?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966706425490357?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966653402162326?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966566715504328?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966521775508822?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966476808846652?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966388225522177?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966375708856762?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966335782194088?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966306918863641?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966263705534629?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/965422742285392?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966245622203104?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966243385536661?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966202212207445?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966189408875392?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966167398877593?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/966134648880868?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/965910925569907?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/965679468926386?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/965634952264171?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/965586232269043?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969491778545155?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969471348547198?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969461055214894?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969456385215361?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969449648549368?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969421088552224?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969417051885961?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969402445220755?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969392405221759?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969383878555945?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969158118578521?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/969022685258731?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/968831421944524?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/968728055288194?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/K14vn/posts/968366765324323?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993967199434727?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993892006108913?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993843276113786?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993793022785478?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993316289499818?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993150319516415?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993217509509696?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/992697889561658?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/992705136227600?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/993099756188138?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/992340396264074?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/992190762945704?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991932829638164?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/992455706252543?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991791036319010?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991721729659274?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991608156337298?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991108859720561?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/991096326388481?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/990926029738844?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/990618286436285?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/thongtinchinhphu/posts/990373226460791?ref=embed_post</t>
+    <t>https://www.facebook.com/K14vn/posts/978847297609603?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/K14vn/posts/978859474275052?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02GqFsseW84Ny9JKv9J8d3WyB1sjucXP3KWi7vpKfZgFrmkrNH8RkXbdXVoDnZmP2Ul?rdid=uOzBUPX5ivpJ3UEj</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0dXuxTmKS9TT5eBFyQw2dZpBYovGaWr5eeQZku5dvfZqHGTUA9yASJjkt8AnGoQbol?rdid=WgxczTy2InBZeAGY#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0g6L98ReFe2E7jG649utmctgB6SbiG9RtSbDzRiMy5cCp6e3LpkKpTi9q3BHtv5pYl?rdid=6fXo6fashJYTOAb9</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02qvdBEJL6K9mFoqonWVdh4dgkhmeHSEbAMgFpjgTtdJ1W6eLepQzmTz6exJ73MBpdl?rdid=g4joSfIKSrUOjEt7#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0ng8TQxCMDn1yJe2pvFeJ67zxQmXYnV4v9vByiYbpB2z7fg6Fcc6tbtbfd3sZxwnWl?rdid=xEYmTQgydrxk1ril#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0inW2YEuyD4soknGuecJinMgAv3E64gRgbuvnAXpesS67vVN7LxMdFuPi1cenxBJzl?rdid=kOJzEqhcpBIoSWjk#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid033Z77RyaBvXPCenHPTE5SaX7fE2bjP8yWjJKpZHKBJmex4pTzrtERCKUYxLwzTLcol?rdid=4MXDWncirRnjlTdU#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582832450794586?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582821347462363?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582780990799732?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582769520800879?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582734497471048?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582699380807893?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582651787479319?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582640317480466?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582631714147993?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02gZXHyffyNet95kb1TJSjUuEV2ayomau9J1YGfF6J9dRku73XDjTaQUzmwKqP7XtJl?rdid=BJfCJtXzkQR6UvMP</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid023XuX8Covz7UfYoa5iKKD8XWDon68EWcm6HXjiSrpM9LFGVQRzoBthcfdPKS9Ke5Kl?rdid=Vdbos1Uv6iCh5YRb#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid09cDe5zqwVrVxF9anZwFxm8Yp3c6y3vjpiHBZAN7JdZmFS9WJ2dLSA7EUSKXvioDdl?rdid=n9612TDHV2ZjnkNx</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0fKZ8BLCf1Y8LuwHTvv6ikDVkEJZbnhhS8PiBZxkzSf5p58saJ8qtwjEcTAH7gtK6l?rdid=6EhQquUUfP7ZytPZ</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02zY3Qo6jTkTvXWyAi2h5vG3LyTun1JHNVMbJqpCCqNZwUJsgDSb46yacEvtDVKB1Xl?rdid=DZi1qyNKGFe9Fxay#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0239C1W3potBMMc39U6UEQQK1huz9KZ42kfMKVUi5yhJQoM7NxVUqKBauNDkgmUdjvl?rdid=T6fKv4Q7JI7HxG3o#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02Sm83QKDjMUGurY6MvgH88XwALn3xzHjAJwFQ1zEMy7YUaQQnobs6j8VR5dadXBEgl?rdid=ybgH4oMUnvHSN3sU</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02YzcB3ukeQxrhmh5zQoNPqHo1YysAw1RoDoTzRMJi7S7PBzsRi6f7Hmckecu3cDgwl?rdid=9sfQRH5wiFVXamC7</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid05nxbxdPeThLLj3QKShRaFoBbTsUdLZxEuCZ7EMf26T5SXszwhXgH9Sf1bL4PqDABl?rdid=Vtj6ioUnIRuRdFpK</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582435514167613?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582382027506295?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582418364169328?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/582092200868611?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581886037555894?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581864334224731?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581812774229887?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02Qy3ZbAxWceTpDgoj1oJKLtY1YbgYXW8aKQufJv5nGWkHNdasXBovyZdd9aCzidsYl?rdid=wuzvuOA4liuc6nBp</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0MvTF4gT6sgNwUBHc1ptrwHFWdgscdGzJJcYCh2gdbH9tkzc65L6Hgz1b7yXiFjaXl?rdid=T506zbiv1GEDy272#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0tZxTbJWw22WHhCaSwoiuJCmTZkKZocv9mE7YiM8ZeNTjKjutrkjbaShSd3w1Xw9Zl?rdid=rF434vu2ddNQRffr</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid031dvwAttigePgUm4Ad5FyojmU7tm4Tr2qoVKFgn8LaF4Q6teUoFV925UBUdiyTeVVl?rdid=gCnVnZBbn8V7GP3G</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0iZWFz86njQCQUDHhwySrfi2UJgxgX7CUpeQGLmFQgswVQAjj7BPfUzDoNkzQVnYUl?rdid=e0fc9FoWvvFxxdeq#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581770297567468?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581747840903047?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581708224240342?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581490030928828?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581431880934643?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581380300939801?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581254167619081?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581231584288006?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581214594289705?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581198927624605?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581122917632206?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid08y63NKsfgzGVnHrpyhduffCQ6pKAMfb3ktwMSNYLYB1a48fE9Q9ZyFwPY9BgcDcYl?rdid=1DXjWo7bMkosUSMz#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0AT33dprJKKJSNNcfdnb1Jr1ntJipKZSMzrwS33jAjNUyE22L4zHdonHk6wgiWPLCl?rdid=5tm6fG3mIGI8uGi4</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid031SuBWRfUvHk1k7DUp9VvR3UYBfScLrGSzmr1LCkeSozphqHP1uvMqbKrHdtDPWwvl?rdid=uSZIq91IuGkb7l2Y#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid06ekzX3YsoBgioW6GmNmNBbRFpcKuDhNnJCVeYUfXxbNrsp7dcXnkCHHM8CD5dWzpl?rdid=JlAM3ZiFcgGmip3g#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0Zr5eNBBpEsnCWfAZCA7kwuCmZd7os5coGwskeBY1s8HMm4XGHKWpAZ69YXckWogDl?rdid=uKB9C1jINmiAvSGZ#</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid02n2n72RBGHes34vBPwmTKFj4Y3pt1psHG7RmEPHi9jKGQE7tuM5ufRwbyhCtL4SJUl?rdid=4EwYdfhLJh8hW8LA</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581105654300599?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581094917635006?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581085930969238?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581077177636780?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/581029417641556?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580993597645138?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580791070998724?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580642814346883?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580595224351642?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580588674352297?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580580851019746?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580566837687814?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580519671025864?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/pfbid0YScLnz9wg5nCk2Z1RuwuQviyxxzzp9BmEuKNT6ohvwk5r3x8fS3xJ4FJ1h4haJpTl?rdid=ocB8vw8078TW36I6</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580490697695428?ref=embed_post</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/vietnamnet.vn/posts/580419001035931?ref=embed_post</t>
   </si>
 </sst>
 </file>
@@ -252,16 +258,10 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -737,133 +737,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -871,10 +871,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1410,10 +1410,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A71"/>
+  <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15"/>
@@ -1579,12 +1579,12 @@
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" s="1" customFormat="1" spans="1:1">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1610,173 +1610,188 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="2"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A34" r:id="rId1" display="https://www.facebook.com/K14vn/posts/965586232269043?ref=embed_post"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>